<commit_message>
Updates from France and Sweden
</commit_message>
<xml_diff>
--- a/i18n/excel_from_translation/Best4Soil.Support.Tools.xlsx
+++ b/i18n/excel_from_translation/Best4Soil.Support.Tools.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26006"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rskgroup.sharepoint.com/sites/IPMDecisions274/Shared Documents/WP2/Translation files/Release-2022-12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="11_047FEA9A8CAA5E77CFE32BDFB281A0CF32A07134" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D068C6D2-C5DD-4487-93B0-842BF62868AE}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="11_047FEA9A8CAA5E77CFE32BDFB281A0CF32A07134" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6AA4026-02E9-4A21-AC9E-6C6D51ACF64D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
   <si>
     <t>KEY</t>
   </si>
@@ -103,6 +103,9 @@
     <t>gr¨</t>
   </si>
   <si>
+    <t>fr</t>
+  </si>
+  <si>
     <t>Best4Soil.Support.Tools.1_0.name</t>
   </si>
   <si>
@@ -124,6 +127,9 @@
     <t>Best4Soil DSS για νηματώδεις και ασθένειες του εδάφους</t>
   </si>
   <si>
+    <t>OAD Best4Soil pour les nématodes et les maladies telluriques</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
@@ -131,9 +137,6 @@
   </si>
   <si>
     <t>lt</t>
-  </si>
-  <si>
-    <t>fr</t>
   </si>
   <si>
     <t>gr</t>
@@ -159,6 +162,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">THE PEST: Plant parasitic nematodes can cause serious damage to crop yield and crop quality. Important groups of plant parasitic nematodes are: cyst nematodes, root-knot nematodes, root-lesions nematodes, stem nematodes and free living nematodes. THE DECISION: Nematodes can best be managed by healthy crop rotations, as crops and crop varieties have a different host status for nematodes. Alternating host and non-host crops or varieties lowers infestation rates in the soil. THE MODEL: The model databases contain information about susceptibility and tolerance of 70 crops to 32 nematodes. The databases are neither soil-specific nor country-specific. PARAMETERS: </t>
     </r>
@@ -167,6 +171,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>The model uses crops, including green manure crops, and crop rotation. T</t>
     </r>
@@ -175,12 +180,60 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>his farm specific input has to be provided by the user. SOURCE: Created by H2020 project Best4Soil, based on the Dutch model www.aaltjesschema.nl, developed by Wageningen University and Research. ASSUMPTIONS: The model gives risk information, assuming that the user selected plant parasitic nematodes are present in the field.</t>
     </r>
   </si>
   <si>
-    <t>DE PEST: Plantaardige parasitaire aaltjes kunnen ernstige schade toebrengen aan de opbrengst en de kwaliteit van gewassen. Belangrijke groepen van plantenparasitaire aaltjes zijn: cysteaaltjes, wortelknobbelaaltjes, wortellesieaaltjes, stengelaaltjes en vrijlevende aaltjes. HET BESLUIT: Nematoden kunnen het best worden beheerd door gezonde vruchtwisselingen, aangezien gewassen en gewasvariëteiten een verschillende gastheerstatus hebben voor nematoden. Het afwisselen van gastheer en niet-gastheer gewassen of rassen verlaagt de besmettingsgraad in de bodem. HET MODEL: De databanken bevatten informatie over de gevoeligheid en tolerantie van 70 gewassen voor 32 nematoden. De databases zijn niet bodemspecifiek en landspecifiek. PARAMETERS: Het model gebruikt informatie over gewassen, inclusief groenbemestingsgewassen, en vruchtwisseling. Deze bedrijfsspecifieke gegevens moeten door de gebruiker worden verstrekt. BRON: Gemaakt door H2020-project Best4Soil, gebaseerd op het Nederlandse model www.aaltjesschema.nl, ontwikkeld door Wageningen Universiteit en Research. AANNAMES: Het model geeft risico-informatie, ervan uitgaande dat de door de gebruiker geselecteerde plantenparasitaire nematoden op het veld aanwezig zijn.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DE PLAAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">: Plantaardige parasitaire aaltjes kunnen ernstige schade toebrengen aan de opbrengst en de kwaliteit van gewassen. Belangrijke groepen van plantenparasitaire aaltjes zijn: cysteaaltjes, wortelknobbelaaltjes, wortellesieaaltjes, stengelaaltjes en vrijlevende aaltjes. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DE BESLISSING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: Nematoden kunnen het best worden beheerd door gezonde vruchtwisselingen, aangezien gewassen en gewasvariëteiten een verschillende gastheerstatus hebben voor nematoden. Het afwisselen van gastheer en niet-gastheer gewassen of rassen verlaagt de besmettingsgraad in de bodem. HET MODEL: De databanken bevatten informatie over de gevoeligheid en tolerantie van 70 gewassen voor 32 nematoden. De databases zijn niet bodemspecifiek en landspecifiek. PARAMETERS: Het model gebruikt informatie over gewassen, inclusief groenbemestingsgewasse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>n en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> vruchtwisseling. Deze bedrijfsspecifieke gegevens moeten door de gebruiker worden verstrekt. BRON: Gemaakt door H2020-project Best4Soil, gebaseerd op het Nederlandse model www.aaltjesschema.nl, ontwikkeld door Wageningen Universiteit en Research. AANNAMES: Het model geeft risico-informatie, ervan uitgaande dat de door de gebruiker geselecteerde plantenparasitaire nematoden op het veld aanwezig zijn.</t>
+    </r>
   </si>
   <si>
     <t>SCHADERREGER: Pflanzenparasitische Nematoden können den Ertrag und die Qualität von Kulturpflanzen ernsthaft schädigen. Wichtige Gruppen von pflanzenparasitären Nematoden sind: Zystennematoden, Wurzelknotennematoden, Wurzelläsionsnematoden, Stängelnematoden und freilebende Nematoden. ENTSCHEIDUNG: Nematoden lassen sich am besten durch eine gesunde Fruchtfolge bekämpfen, da die Kulturen und Pflanzensorten einen unterschiedlichen Wirtsstatus für Nematoden haben. Der Wechsel zwischen Wirtspflanzen und Nicht-Wirtspflanzen oder -sorten senkt die Befallsrate im Boden. MODELL: Die Datenbasis des Modells enthält Informationen über die Anfälligkeit und Toleranz von 70 Kulturpflanzen gegenüber 32 Nematoden. Die Datenbasis ist weder bodenspezifisch noch länderspezifisch. PARAMETER: Die Ertragsrisiken basieren auf den Kulturen, einschließlich Gründüngungskulturen, und der Fruchtfolge. Diese betriebsspezifischen Angaben müssen vom Nutzer gemacht werden. QUELLE: Erstellt im Rahmen des H2020-Projekts Best4Soil auf der Grundlage des niederländischen Modells www.aaltjesschema.nl, das von Wageningen University and Research entwickelt wurde. ANNAHMEN: Das Modell liefert Risikoinformationen unter der Annahme, dass die vom Benutzer ausgewählten pflanzenparasitären Nematoden auf dem Feld vorhanden sind.</t>
@@ -325,7 +378,30 @@
     <t xml:space="preserve">  THE PEST: Soil-borne pathogens can cause serious damage to crop yield and quality. Major groups of such pathogens are: Fusarium, Phoma, Phomopsis, Phytophthora, Pythium, Rhizoctonia and Sclerotinia. Soil-borne pathogens can often be managed by crop rotations, as they infect only certain crop species and usually decline in the absence of a host crop.  A rotation containing non-host crops or varieties can lower infestation rates in the soil. THE MODEL: The model databases contain information about susceptibility and tolerance of 70 crops to 135 pathogens. PARAMETERS: The model uses crops, including green manure crops, and crop rotation. This farm specific input has to be provided by the user. SOURCE: Created by H2020 project Best4Soil, analogue to the Dutch model www.aaltjesschema.nl, developed by Wageningen University and Research. ASSUMPTIONS: The model gives risk information, assuming that the user selected plant pathogens are present in the field. At the moment, the databases are neither soil-specific, nor country-specific. This means that the crop schemes are identical for different soil types and countries. At this moment there is insufficient country-specific information on host status and sensitivity to crop damage per crop to make the database country-specific. The same is the case for soil type specific information. Because soil type plays a role in the occurrence of  soil pathogens, the soil type selection button has been built in to enable soil type specific schemes in the future. </t>
   </si>
   <si>
-    <t xml:space="preserve"> DE ZIEKTE: Bodemgebonden ziektes kunnen ernstige schade toebrengen aan de opbrengst en de kwaliteit van de gewassen. Belangrijke groepen van dergelijke ziekteverwekkers zijn: Fusarium, Phoma, Phomopsis, Phytophthora, Pythium, Rhizoctonia en Sclerotinia. Bodemgebonden ziektes kunnen vaak worden beheerst door gewasrotaties, aangezien zij slechts bepaalde gewassoorten infecteren en gewoonlijk afnemen bij afwezigheid van een waardplant.  Een rotatie met niet-gastheergewassen of -variëteiten kan de besmettingsgraad in de bodem verlagen. HET MODEL: De modeldatabases bevatten informatie over de gevoeligheid en tolerantie van 70 gewassen voor 135 ziekteverwekkers. PARAMETERS: Het model gebruikt gewassen, inclusief groenbemesters, en vruchtwisseling. Deze bedrijfsspecifieke informatie moet door de gebruiker worden verstrekt. BRON: Gemaakt door H2020-project Best4Soil, analoog aan het Nederlandse model www.aaltjesschema.nl, ontwikkeld door Wageningen Universiteit en Research. AANNAMES: Het model geeft risico-informatie, ervan uitgaande dat de door de gebruiker geselecteerde plantenziekteverwekkers in het veld aanwezig zijn. Momenteel zijn de databases noch bodemspecifiek, noch landspecifiek. Dit betekent dat de gewasschema's identiek zijn voor verschillende bodemtypes en landen. Op dit moment is er onvoldoende landspecifieke informatie over gastheerstatus en gevoeligheid voor gewasschade per gewas om de database landspecifiek te maken. Hetzelfde geldt voor de bodemtype-specifieke informatie. Omdat bodemtype een rol speelt bij het voorkomen van bodempathogenen, is de bodemtypeselectieknop ingebouwd om in de toekomst bodemtypespecifieke schema's mogelijk te maken. </t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> DE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PLAAG:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> Bodemgebonden ziektes kunnen ernstige schade toebrengen aan de opbrengst en de kwaliteit van de gewassen. Belangrijke groepen van dergelijke ziekteverwekkers zijn: Fusarium, Phoma, Phomopsis, Phytophthora, Pythium, Rhizoctonia en Sclerotinia. Bodemgebonden ziektes kunnen vaak worden beheerst door gewasrotaties, aangezien zij slechts bepaalde gewassoorten infecteren en gewoonlijk afnemen bij afwezigheid van een waardplant.  Een rotatie met niet-gastheergewassen of -variëteiten kan de besmettingsgraad in de bodem verlagen. HET MODEL: De modeldatabases bevatten informatie over de gevoeligheid en tolerantie van 70 gewassen voor 135 ziekteverwekkers. PARAMETERS: Het model gebruikt gewassen, inclusief groenbemesters, en vruchtwisseling. Deze bedrijfsspecifieke informatie moet door de gebruiker worden verstrekt. BRON: Gemaakt door H2020-project Best4Soil, analoog aan het Nederlandse model www.aaltjesschema.nl, ontwikkeld door Wageningen Universiteit en Research. AANNAMES: Het model geeft risico-informatie, ervan uitgaande dat de door de gebruiker geselecteerde plantenziekteverwekkers in het veld aanwezig zijn. Momenteel zijn de databases noch bodemspecifiek, noch landspecifiek. Dit betekent dat de gewasschema's identiek zijn voor verschillende bodemtypes en landen. Op dit moment is er onvoldoende landspecifieke informatie over gastheerstatus en gevoeligheid voor gewasschade per gewas om de database landspecifiek te maken. Hetzelfde geldt voor de bodemtype-specifieke informatie. Omdat bodemtype een rol speelt bij het voorkomen van bodempathogenen, is de bodemtypeselectieknop ingebouwd om in de toekomst bodemtypespecifieke schema's mogelijk te maken. </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">SCHADERREGER: Bodenpathogene können den Ertrag und die Qualität der Ernte ernsthaft beeinträchtigen. Die wichtigsten Gruppen solcher Krankheitserreger sind: Fusarium, Phoma, Phomopsis, Phytophthora, Pythium, Rhizoctonia und Sclerotinia. Bodenbürtige Krankheitserreger lassen sich häufig durch Fruchtfolgen in den Griff bekommen, da sie nur bestimmte Pflanzenarten befallen und in der Regel ohne Wirtspflanzen zurückgehen.  Eine Fruchtfolge mit Nicht-Wirtspflanzen oder -sorten kann die Befallsrate im Boden senken. MODELL: Die Modelldatenbank enthält Informationen über die Anfälligkeit und Toleranz von 70 Kulturpflanzen gegenüber 135 Krankheitserregern. PARAMETER: Das Modell verwendet Kulturen, einschließlich Gründüngungskulturen, und Fruchtfolgen. Diese betriebsspezifischen Eingaben müssen vom Benutzer bereitgestellt werden. QUELLE: Erstellt im Rahmen des H2020-Projekts Best4Soil, analog zum niederländischen Modell www.aaltjesschema.nl, das von das von Wageningen University and Research entwickelt wurde. ANNAHMEN: Das Modell liefert Risikoinformationen unter der Annahme, dass die vom Benutzer ausgewählten Pflanzenpathogene auf dem Feld vorhanden sind. Zurzeit ist die Datenbank weder boden- noch länderspezifisch. Das bedeutet, dass die Anbauschemata für verschiedene Bodentypen und Länder identisch sind. Gegenwärtig gibt es keine ausreichenden länderspezifischen Informationen über den Wirtsstatus und die Empfindlichkeit gegenüber Pflanzenschäden pro Kultur, um die Datenbank länderspezifisch zu gestalten. Das Gleiche gilt für bodenartspezifische Informationen. Da die Bodenart beim Auftreten von Bodenpathogenen eine Rolle spielt, wurde die Schaltfläche zur Auswahl der Bodenart eingebaut, um in Zukunft bodenartspezifische Schemata zu ermöglichen. </t>
@@ -360,6 +436,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ŠKODLJIVI ORGANIZMI: Patogeni, ki se prenašajo s tlemi, lahko povzročijo resno škodo na pridelku in kakovosti pridelka. Glavne skupine takšnih patogenov so: </t>
     </r>
@@ -369,6 +446,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Fusarium, Phoma, Phomopsis, Phytophthora, Pythium, Rhizoctonia in Sclerotinia</t>
     </r>
@@ -377,6 +455,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>. Talne patogene lahko pogosto obvladujemo s kolobarjenjem, saj okužijo le nekatere vrste poljščin in običajno propadejo, če ni gostiteljske rastline. Kolobar, ki vsebuje poljščine ali sorte, ki niso gostiteljice, lahko zmanjša stopnjo okužbe v tleh. MODEL: Podatkovne zbirke modela vsebujejo informacije o občutljivosti in toleranci 70 poljščin na 135 patogenov. PARAMETRI: Model uporablja posevke, vključno s posevki za zeleno gnojenje, in kolobarjenje. Te vhodne podatke za posamezno kmetijo mora zagotoviti uporabnik. VIR: Razvit je bil v okviru projekta H2020 Best4Soil, na podlagi nizozemskega modela www.aaltjesschema.nl, ki ga je razvil Wageningen university &amp; research. PREDPOSTAVKE: Model ponuja informacije o tveganju ob predpostavki, da so na polju prisotni uporabniško izbrani rastlinski patogeni. Trenutno podatkovne zbirke niso prilagojene niti za posamezna tla niti za posamezno državo. To pomeni, da so sheme posevkov enake za različne vrste tal in države. Zaenkrat ni na voljo dovolj informacij o stanju gostitelja in občutljivosti na poškodbe poljščin za posamezno državo, da bi bila zbirka podatkov prilagojena posamezni državi. Enako velja za informacije o vrsti tal. Ker ima tip tal pomembno vlogo pri pojavu talnih patogenov, je bil vgrajen gumb za izbiro tipa tal, ki bo v prihodnosti omogočil sheme za posamezne tipe tal.</t>
     </r>
@@ -467,7 +546,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -487,9 +566,22 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -498,6 +590,13 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -553,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -587,6 +686,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,21 +1027,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="38.140625" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -966,28 +1070,34 @@
       <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1000,11 +1110,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="43.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="59.42578125" style="3" customWidth="1"/>
@@ -1042,227 +1152,227 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="337.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="C2" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="60.75">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="57.6">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="30.75">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="28.9">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="45.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="28.9">
       <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="45.75">
+    </row>
+    <row r="6" spans="1:17" ht="43.15">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="45.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="28.9">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="45.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="43.15">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="45.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="28.9">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="45.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="43.15">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="45.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="28.9">
       <c r="A11" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="45.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="43.15">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="45.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="28.9">
       <c r="A13" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="45.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="43.15">
       <c r="A14" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="106.5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="100.9">
       <c r="A15" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1270,15 +1380,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="62.28515625" customWidth="1"/>
     <col min="2" max="2" width="81.85546875" customWidth="1"/>
-    <col min="3" max="3" width="58" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="7" width="8.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="47.85546875" style="2" customWidth="1"/>
@@ -1305,187 +1415,187 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="293.25" customHeight="1">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="45.75">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="43.15">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:16" ht="198">
+    <row r="15" spans="1:16" ht="172.9">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1496,6 +1606,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="f0f33890-2782-435d-9951-89eaf76ec08c">
@@ -1506,15 +1625,6 @@
     <TaxCatchAll xmlns="49b2234f-12e0-4bdf-b627-3d078507bec9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1778,11 +1888,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{442F9C8F-405C-4F57-BF5E-08A1AB6E2DA9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBF30B5-13F8-4ED4-822A-2F6B5ABD79E3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBF30B5-13F8-4ED4-822A-2F6B5ABD79E3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{442F9C8F-405C-4F57-BF5E-08A1AB6E2DA9}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>